<commit_message>
Change Price Scrape file to package. Import and loop cleanly through each entry in Grocery List.xlsx
</commit_message>
<xml_diff>
--- a/Grocery List.xlsx
+++ b/Grocery List.xlsx
@@ -5,15 +5,16 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Sync\Shared Folder\Groceries and Takeout\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\miche\PycharmProjects\GroceryCalculation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3C37651-D4DF-484A-BAC5-C220448D70BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8284AB2A-E83B-4E67-8D02-0577403C873B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14355" yWindow="4140" windowWidth="17295" windowHeight="15345" xr2:uid="{1EE981F6-777C-4836-83F6-183769BB43C2}"/>
+    <workbookView xWindow="768" yWindow="768" windowWidth="17280" windowHeight="8964" activeTab="1" xr2:uid="{1EE981F6-777C-4836-83F6-183769BB43C2}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sprouts" sheetId="1" r:id="rId1"/>
+    <sheet name="Hy-Vee" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="37">
   <si>
     <t>Quantity</t>
   </si>
@@ -47,9 +48,6 @@
   </si>
   <si>
     <t>Notes</t>
-  </si>
-  <si>
-    <t>Sprouts</t>
   </si>
   <si>
     <t>Pink Lady Apples</t>
@@ -158,13 +156,20 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
   </numFmts>
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="1"/>
+      <name val="Bierstadt"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -187,9 +192,18 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -504,296 +518,335 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9651953D-2BB0-4628-B9A4-C6D08C7039C7}">
-  <dimension ref="A1:E39"/>
+  <dimension ref="A1:E35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="A38" sqref="A36:XFD38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="79.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="56.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="79.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="56.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
+      <c r="B1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="3" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>2</v>
+      </c>
       <c r="B3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" s="1">
+        <v>3.99</v>
+      </c>
+      <c r="D3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E3" s="1"/>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>7</v>
+      </c>
+      <c r="B4" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>2</v>
-      </c>
-      <c r="B4" t="s">
-        <v>11</v>
-      </c>
       <c r="C4" s="1">
-        <v>3.99</v>
+        <v>0.53</v>
       </c>
       <c r="D4" t="s">
-        <v>14</v>
-      </c>
-      <c r="E4" s="1"/>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="B5" t="s">
         <v>5</v>
       </c>
       <c r="C5" s="1">
-        <v>0.53</v>
-      </c>
-      <c r="D5" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+        <v>2.4900000000000002</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>1</v>
       </c>
       <c r="B6" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="C6" s="1">
         <v>2.4900000000000002</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="B7" t="s">
         <v>12</v>
       </c>
       <c r="C7" s="1">
-        <v>2.4900000000000002</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="D7" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="B8" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="C8" s="1">
-        <v>1</v>
+        <v>3.49</v>
       </c>
       <c r="D8" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B9" t="s">
+        <v>14</v>
+      </c>
+      <c r="C9" s="1">
+        <v>0.98</v>
+      </c>
+      <c r="D9" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>0.5</v>
+      </c>
+      <c r="B10" t="s">
+        <v>17</v>
+      </c>
+      <c r="C10" s="1">
+        <v>3.99</v>
+      </c>
+      <c r="D10" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <v>1</v>
+      </c>
+      <c r="B11" t="s">
         <v>20</v>
       </c>
-      <c r="C9" s="1">
-        <v>3.49</v>
-      </c>
-      <c r="D9" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10">
-        <v>1</v>
-      </c>
-      <c r="B10" t="s">
-        <v>15</v>
-      </c>
-      <c r="C10" s="1">
-        <v>0.98</v>
-      </c>
-      <c r="D10" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11">
-        <v>0.5</v>
-      </c>
-      <c r="B11" t="s">
-        <v>18</v>
-      </c>
       <c r="C11" s="1">
-        <v>3.99</v>
+        <v>2.5</v>
       </c>
       <c r="D11" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>1</v>
       </c>
       <c r="B12" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C12" s="1">
-        <v>2.5</v>
+        <v>1.5</v>
       </c>
       <c r="D12" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>1</v>
       </c>
       <c r="B13" t="s">
-        <v>23</v>
+        <v>35</v>
       </c>
       <c r="C13" s="1">
-        <v>1.5</v>
+        <v>1.1499999999999999</v>
       </c>
       <c r="D13" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A14">
+        <v>1</v>
+      </c>
+      <c r="B14" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14">
-        <v>1</v>
-      </c>
-      <c r="B14" t="s">
-        <v>36</v>
-      </c>
       <c r="C14" s="1">
-        <v>1.1499999999999999</v>
+        <v>1.99</v>
       </c>
       <c r="D14" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15">
-        <v>1</v>
-      </c>
-      <c r="B15" t="s">
         <v>25</v>
       </c>
-      <c r="C15" s="1">
-        <v>1.99</v>
-      </c>
-      <c r="D15" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B21" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22">
-        <v>3</v>
-      </c>
-      <c r="B22" t="s">
-        <v>8</v>
-      </c>
-      <c r="C22" s="1">
-        <v>3.49</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23">
-        <v>2</v>
-      </c>
-      <c r="B23" t="s">
-        <v>28</v>
-      </c>
-      <c r="C23" s="1">
-        <v>1.99</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24">
-        <v>1</v>
-      </c>
-      <c r="B24" t="s">
-        <v>29</v>
-      </c>
-      <c r="C24" s="1">
-        <v>2.69</v>
-      </c>
-      <c r="D24" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25">
-        <v>1</v>
-      </c>
-      <c r="B25" t="s">
-        <v>30</v>
-      </c>
-      <c r="C25" s="1">
-        <v>1.99</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26">
-        <v>1</v>
-      </c>
-      <c r="B26" t="s">
-        <v>31</v>
-      </c>
-      <c r="C26" s="1">
-        <v>7.99</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27">
-        <v>1</v>
-      </c>
-      <c r="B27" t="s">
-        <v>32</v>
-      </c>
-      <c r="C27" s="1">
-        <v>3.79</v>
-      </c>
-      <c r="D27" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="36" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="37" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B37" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="38" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B38" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="39" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B39" t="s">
-        <v>17</v>
-      </c>
-    </row>
+    </row>
+    <row r="35" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7AB05AA7-9324-4DA2-8CB2-01E0BB5DD03F}">
+  <dimension ref="A1:D12"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A10" sqref="A10:XFD12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="41.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="5.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="24.21875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="2"/>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>3</v>
+      </c>
+      <c r="B3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="1">
+        <v>3.49</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C4" s="1">
+        <v>1.99</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>1</v>
+      </c>
+      <c r="B5" t="s">
+        <v>28</v>
+      </c>
+      <c r="C5" s="1">
+        <v>2.69</v>
+      </c>
+      <c r="D5" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>1</v>
+      </c>
+      <c r="B6" t="s">
+        <v>29</v>
+      </c>
+      <c r="C6" s="1">
+        <v>1.99</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>1</v>
+      </c>
+      <c r="B7" t="s">
+        <v>30</v>
+      </c>
+      <c r="C7" s="1">
+        <v>7.99</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>1</v>
+      </c>
+      <c r="B8" t="s">
+        <v>31</v>
+      </c>
+      <c r="C8" s="1">
+        <v>3.79</v>
+      </c>
+      <c r="D8" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B10" t="s">
+        <v>9</v>
+      </c>
+      <c r="C10" s="1"/>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B11" t="s">
+        <v>8</v>
+      </c>
+      <c r="C11" s="1"/>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B12" t="s">
+        <v>16</v>
+      </c>
+      <c r="C12" s="1"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:D1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Change store locator function code in response to changes on Sprouts' site
</commit_message>
<xml_diff>
--- a/Grocery List.xlsx
+++ b/Grocery List.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="17880" yWindow="1440" windowWidth="17295" windowHeight="15345" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="18570" yWindow="2130" windowWidth="17295" windowHeight="15345" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sprouts" sheetId="1" state="visible" r:id="rId1"/>
@@ -128,39 +128,6 @@
     </indexedColors>
   </colors>
 </styleSheet>
-</file>
-
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<wsDr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
-  <oneCellAnchor>
-    <from>
-      <col>5</col>
-      <colOff>0</colOff>
-      <row>1</row>
-      <rowOff>0</rowOff>
-    </from>
-    <ext cx="619125" cy="619125"/>
-    <pic>
-      <nvPicPr>
-        <cNvPr id="1" name="Image 1" descr="Picture"/>
-        <cNvPicPr/>
-      </nvPicPr>
-      <blipFill>
-        <a:blip cstate="print" r:embed="rId1"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </blipFill>
-      <spPr>
-        <a:prstGeom prst="rect"/>
-        <a:ln>
-          <a:prstDash val="solid"/>
-        </a:ln>
-      </spPr>
-    </pic>
-    <clientData/>
-  </oneCellAnchor>
-</wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -483,7 +450,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
@@ -492,7 +459,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F2" sqref="F2"/>
+      <selection pane="bottomLeft" activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
@@ -544,14 +511,7 @@
           <t>Pink Lady Apples</t>
         </is>
       </c>
-      <c r="C2" s="2" t="n">
-        <v>0.6</v>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>https://assets-prd-spr.unataops.com/web/product_small/8fc77215a3ec068000e57b3e1fd5d3b7a46527ce.jpg</t>
-        </is>
-      </c>
+      <c r="C2" s="2" t="n"/>
     </row>
     <row r="3" ht="66" customHeight="1"/>
     <row r="4" ht="66" customHeight="1"/>
@@ -604,7 +564,6 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait"/>
-  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Fixed scrapers to reflect changes on Sprouts site Now to work on Excel implementation
</commit_message>
<xml_diff>
--- a/Grocery List.xlsx
+++ b/Grocery List.xlsx
@@ -1,36 +1,74 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
+  <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Sync\Shared Folder\Groceries and Takeout\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE733A5F-9374-46DE-A321-A899793F9D60}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="18570" yWindow="2130" windowWidth="17295" windowHeight="15345" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView xWindow="18570" yWindow="2130" windowWidth="17295" windowHeight="15345" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sprouts" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="Hy-Vee" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="Sprouts" sheetId="1" r:id="rId1"/>
+    <sheet name="Hy-Vee" sheetId="2" r:id="rId2"/>
   </sheets>
-  <definedNames/>
-  <calcPr calcId="0" fullCalcOnLoad="1"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="9">
+  <si>
+    <t>Quantity</t>
+  </si>
+  <si>
+    <t>Item</t>
+  </si>
+  <si>
+    <t>Price</t>
+  </si>
+  <si>
+    <t>Image Link</t>
+  </si>
+  <si>
+    <t>Notes</t>
+  </si>
+  <si>
+    <t>Image</t>
+  </si>
+  <si>
+    <t>Pink Lady Apples</t>
+  </si>
+  <si>
+    <t>https://assets-prd-spr.unataops.com/web/product_small/8fc77215a3ec068000e57b3e1fd5d3b7a46527ce.jpg</t>
+  </si>
+  <si>
+    <t>Corn</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
   </numFmts>
-  <fonts count="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <color theme="1"/>
-      <sz val="11"/>
       <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill/>
+      <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -49,84 +87,25 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="3">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <colors>
-    <indexedColors>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008000"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00808000"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="00C0C0C0"/>
-      <rgbColor rgb="00808080"/>
-      <rgbColor rgb="009999FF"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00FFFFCC"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00660066"/>
-      <rgbColor rgb="00FF8080"/>
-      <rgbColor rgb="000066CC"/>
-      <rgbColor rgb="00CCCCFF"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="0000CCFF"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00CCFFCC"/>
-      <rgbColor rgb="00FFFF99"/>
-      <rgbColor rgb="0099CCFF"/>
-      <rgbColor rgb="00FF99CC"/>
-      <rgbColor rgb="00CC99FF"/>
-      <rgbColor rgb="00FFCC99"/>
-      <rgbColor rgb="003366FF"/>
-      <rgbColor rgb="0033CCCC"/>
-      <rgbColor rgb="0099CC00"/>
-      <rgbColor rgb="00FFCC00"/>
-      <rgbColor rgb="00FF9900"/>
-      <rgbColor rgb="00FF6600"/>
-      <rgbColor rgb="00666699"/>
-      <rgbColor rgb="00969696"/>
-      <rgbColor rgb="00003366"/>
-      <rgbColor rgb="00339966"/>
-      <rgbColor rgb="00003300"/>
-      <rgbColor rgb="00333300"/>
-      <rgbColor rgb="00993300"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00333399"/>
-      <rgbColor rgb="00333333"/>
-    </indexedColors>
-  </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -450,117 +429,106 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:F2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:F50"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D4" sqref="D4"/>
+      <selection pane="bottomLeft" activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col width="16" bestFit="1" customWidth="1" min="2" max="2"/>
-    <col width="10.140625" bestFit="1" customWidth="1" style="1" min="3" max="3"/>
-    <col width="98.85546875" bestFit="1" customWidth="1" min="4" max="4"/>
-    <col width="9.42578125" customWidth="1" min="6" max="6"/>
+    <col min="2" max="2" width="16" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="98.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>Quantity</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>Item</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>Price</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>Image Link</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>Notes</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>Image</t>
-        </is>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
       </c>
     </row>
-    <row r="2" ht="66" customHeight="1">
-      <c r="A2" t="n">
+    <row r="2" spans="1:6" ht="66" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2">
         <v>1</v>
       </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>Pink Lady Apples</t>
-        </is>
-      </c>
-      <c r="C2" s="2" t="n"/>
+      <c r="B2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="2"/>
     </row>
-    <row r="3" ht="66" customHeight="1"/>
-    <row r="4" ht="66" customHeight="1"/>
-    <row r="5" ht="66" customHeight="1"/>
-    <row r="6" ht="66" customHeight="1"/>
-    <row r="7" ht="66" customHeight="1"/>
-    <row r="8" ht="66" customHeight="1"/>
-    <row r="9" ht="66" customHeight="1"/>
-    <row r="10" ht="66" customHeight="1"/>
-    <row r="11" ht="66" customHeight="1"/>
-    <row r="12" ht="66" customHeight="1"/>
-    <row r="13" ht="66" customHeight="1"/>
-    <row r="14" ht="66" customHeight="1"/>
-    <row r="15" ht="66" customHeight="1"/>
-    <row r="16" ht="66" customHeight="1"/>
-    <row r="17" ht="66" customHeight="1"/>
-    <row r="18" ht="66" customHeight="1"/>
-    <row r="19" ht="66" customHeight="1"/>
-    <row r="20" ht="66" customHeight="1"/>
-    <row r="21" ht="66" customHeight="1"/>
-    <row r="22" ht="66" customHeight="1"/>
-    <row r="23" ht="66" customHeight="1"/>
-    <row r="24" ht="66" customHeight="1"/>
-    <row r="25" ht="66" customHeight="1"/>
-    <row r="26" ht="66" customHeight="1"/>
-    <row r="27" ht="66" customHeight="1"/>
-    <row r="28" ht="66" customHeight="1"/>
-    <row r="29" ht="66" customHeight="1"/>
-    <row r="30" ht="66" customHeight="1"/>
-    <row r="31" ht="66" customHeight="1"/>
-    <row r="32" ht="66" customHeight="1"/>
-    <row r="33" ht="66" customHeight="1"/>
-    <row r="34" ht="66" customHeight="1"/>
-    <row r="35" ht="66" customHeight="1"/>
-    <row r="36" ht="66" customHeight="1"/>
-    <row r="37" ht="66" customHeight="1"/>
-    <row r="38" ht="66" customHeight="1"/>
-    <row r="39" ht="66" customHeight="1"/>
-    <row r="40" ht="66" customHeight="1"/>
-    <row r="41" ht="66" customHeight="1"/>
-    <row r="42" ht="66" customHeight="1"/>
-    <row r="43" ht="66" customHeight="1"/>
-    <row r="44" ht="66" customHeight="1"/>
-    <row r="45" ht="66" customHeight="1"/>
-    <row r="46" ht="66" customHeight="1"/>
-    <row r="47" ht="66" customHeight="1"/>
-    <row r="48" ht="66" customHeight="1"/>
-    <row r="49" ht="66" customHeight="1"/>
-    <row r="50" ht="66" customHeight="1"/>
+    <row r="3" spans="1:6" ht="66" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="66" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="5" spans="1:6" ht="66" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="6" spans="1:6" ht="66" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="7" spans="1:6" ht="66" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="8" spans="1:6" ht="66" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="9" spans="1:6" ht="66" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="10" spans="1:6" ht="66" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="11" spans="1:6" ht="66" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="12" spans="1:6" ht="66" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="13" spans="1:6" ht="66" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="14" spans="1:6" ht="66" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="15" spans="1:6" ht="66" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="16" spans="1:6" ht="66" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="17" ht="66" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="18" ht="66" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="19" ht="66" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="20" ht="66" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="21" ht="66" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="22" ht="66" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="23" ht="66" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="24" ht="66" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="25" ht="66" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="26" ht="66" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="27" ht="66" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="28" ht="66" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="29" ht="66" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="30" ht="66" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="31" ht="66" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="32" ht="66" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="33" ht="66" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="34" ht="66" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="35" ht="66" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="36" ht="66" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="37" ht="66" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="38" ht="66" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="39" ht="66" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="40" ht="66" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="41" ht="66" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="42" ht="66" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="43" ht="66" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="44" ht="66" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="45" ht="66" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="46" ht="66" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="47" ht="66" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="48" ht="66" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="49" ht="66" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="50" ht="66" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait"/>
@@ -568,71 +536,51 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col width="9.28515625" customWidth="1" min="3" max="3"/>
-    <col width="98.85546875" bestFit="1" customWidth="1" min="4" max="4"/>
+    <col min="3" max="3" width="9.28515625" customWidth="1"/>
+    <col min="4" max="4" width="98.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="41.25" customHeight="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>Quantity</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>Item</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>Price</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>Image Link</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>Notes</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>Image</t>
-        </is>
+    <row r="1" spans="1:6" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" t="n">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2">
         <v>1</v>
       </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>Pink Lady Apples</t>
-        </is>
-      </c>
-      <c r="C2" s="2" t="n">
+      <c r="B2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="2">
         <v>0.6</v>
       </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>https://assets-prd-spr.unataops.com/web/product_small/8fc77215a3ec068000e57b3e1fd5d3b7a46527ce.jpg</t>
-        </is>
+      <c r="D2" t="s">
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update to integration of new code with old code
</commit_message>
<xml_diff>
--- a/Grocery List.xlsx
+++ b/Grocery List.xlsx
@@ -1,74 +1,36 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
-  <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Sync\Shared Folder\Groceries and Takeout\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE733A5F-9374-46DE-A321-A899793F9D60}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="18570" yWindow="2130" windowWidth="17295" windowHeight="15345" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="18570" yWindow="2130" windowWidth="17295" windowHeight="15345" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sprouts" sheetId="1" r:id="rId1"/>
-    <sheet name="Hy-Vee" sheetId="2" r:id="rId2"/>
+    <sheet name="Sprouts" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Hy-Vee" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <definedNames/>
+  <calcPr calcId="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="9">
-  <si>
-    <t>Quantity</t>
-  </si>
-  <si>
-    <t>Item</t>
-  </si>
-  <si>
-    <t>Price</t>
-  </si>
-  <si>
-    <t>Image Link</t>
-  </si>
-  <si>
-    <t>Notes</t>
-  </si>
-  <si>
-    <t>Image</t>
-  </si>
-  <si>
-    <t>Pink Lady Apples</t>
-  </si>
-  <si>
-    <t>https://assets-prd-spr.unataops.com/web/product_small/8fc77215a3ec068000e57b3e1fd5d3b7a46527ce.jpg</t>
-  </si>
-  <si>
-    <t>Corn</t>
-  </si>
-</sst>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
   </numFmts>
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="1">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -87,25 +49,84 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="3">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -429,106 +450,126 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F50"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="16" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="98.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.42578125" customWidth="1"/>
+    <col width="16" bestFit="1" customWidth="1" min="2" max="2"/>
+    <col width="10.140625" bestFit="1" customWidth="1" style="1" min="3" max="3"/>
+    <col width="98.85546875" bestFit="1" customWidth="1" min="4" max="4"/>
+    <col width="9.42578125" customWidth="1" min="6" max="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>Quantity</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>Item</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Price</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>Image Link</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>Notes</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>Image</t>
+        </is>
+      </c>
+    </row>
+    <row r="2" ht="66" customHeight="1">
+      <c r="A2" t="n">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" t="s">
-        <v>5</v>
-      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Pink Lady Apples</t>
+        </is>
+      </c>
+      <c r="C2" s="2" t="n"/>
     </row>
-    <row r="2" spans="1:6" ht="66" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2">
+    <row r="3" ht="66" customHeight="1">
+      <c r="A3" t="n">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C2" s="2"/>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Corn</t>
+        </is>
+      </c>
     </row>
-    <row r="3" spans="1:6" ht="66" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>1</v>
-      </c>
-      <c r="B3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" ht="66" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="5" spans="1:6" ht="66" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="6" spans="1:6" ht="66" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="7" spans="1:6" ht="66" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="8" spans="1:6" ht="66" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="9" spans="1:6" ht="66" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="10" spans="1:6" ht="66" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="11" spans="1:6" ht="66" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="12" spans="1:6" ht="66" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="13" spans="1:6" ht="66" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="14" spans="1:6" ht="66" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="15" spans="1:6" ht="66" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="16" spans="1:6" ht="66" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="17" ht="66" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="18" ht="66" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="19" ht="66" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="20" ht="66" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="21" ht="66" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="22" ht="66" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="23" ht="66" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="24" ht="66" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="25" ht="66" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="26" ht="66" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="27" ht="66" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="28" ht="66" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="29" ht="66" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="30" ht="66" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="31" ht="66" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="32" ht="66" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="33" ht="66" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="34" ht="66" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="35" ht="66" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="36" ht="66" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="37" ht="66" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="38" ht="66" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="39" ht="66" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="40" ht="66" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="41" ht="66" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="42" ht="66" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="43" ht="66" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="44" ht="66" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="45" ht="66" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="46" ht="66" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="47" ht="66" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="48" ht="66" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="49" ht="66" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="50" ht="66" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="4" ht="66" customHeight="1"/>
+    <row r="5" ht="66" customHeight="1"/>
+    <row r="6" ht="66" customHeight="1"/>
+    <row r="7" ht="66" customHeight="1"/>
+    <row r="8" ht="66" customHeight="1"/>
+    <row r="9" ht="66" customHeight="1"/>
+    <row r="10" ht="66" customHeight="1"/>
+    <row r="11" ht="66" customHeight="1"/>
+    <row r="12" ht="66" customHeight="1"/>
+    <row r="13" ht="66" customHeight="1"/>
+    <row r="14" ht="66" customHeight="1"/>
+    <row r="15" ht="66" customHeight="1"/>
+    <row r="16" ht="66" customHeight="1"/>
+    <row r="17" ht="66" customHeight="1"/>
+    <row r="18" ht="66" customHeight="1"/>
+    <row r="19" ht="66" customHeight="1"/>
+    <row r="20" ht="66" customHeight="1"/>
+    <row r="21" ht="66" customHeight="1"/>
+    <row r="22" ht="66" customHeight="1"/>
+    <row r="23" ht="66" customHeight="1"/>
+    <row r="24" ht="66" customHeight="1"/>
+    <row r="25" ht="66" customHeight="1"/>
+    <row r="26" ht="66" customHeight="1"/>
+    <row r="27" ht="66" customHeight="1"/>
+    <row r="28" ht="66" customHeight="1"/>
+    <row r="29" ht="66" customHeight="1"/>
+    <row r="30" ht="66" customHeight="1"/>
+    <row r="31" ht="66" customHeight="1"/>
+    <row r="32" ht="66" customHeight="1"/>
+    <row r="33" ht="66" customHeight="1"/>
+    <row r="34" ht="66" customHeight="1"/>
+    <row r="35" ht="66" customHeight="1"/>
+    <row r="36" ht="66" customHeight="1"/>
+    <row r="37" ht="66" customHeight="1"/>
+    <row r="38" ht="66" customHeight="1"/>
+    <row r="39" ht="66" customHeight="1"/>
+    <row r="40" ht="66" customHeight="1"/>
+    <row r="41" ht="66" customHeight="1"/>
+    <row r="42" ht="66" customHeight="1"/>
+    <row r="43" ht="66" customHeight="1"/>
+    <row r="44" ht="66" customHeight="1"/>
+    <row r="45" ht="66" customHeight="1"/>
+    <row r="46" ht="66" customHeight="1"/>
+    <row r="47" ht="66" customHeight="1"/>
+    <row r="48" ht="66" customHeight="1"/>
+    <row r="49" ht="66" customHeight="1"/>
+    <row r="50" ht="66" customHeight="1"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait"/>
@@ -536,51 +577,71 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col min="3" max="3" width="9.28515625" customWidth="1"/>
-    <col min="4" max="4" width="98.85546875" bestFit="1" customWidth="1"/>
+    <col width="9.28515625" customWidth="1" min="3" max="3"/>
+    <col width="98.85546875" bestFit="1" customWidth="1" min="4" max="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
+    <row r="1" ht="41.25" customHeight="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>Quantity</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>Item</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Price</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>Image Link</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>Notes</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>Image</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="n">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C2" s="2">
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Pink Lady Apples</t>
+        </is>
+      </c>
+      <c r="C2" s="2" t="n">
         <v>0.6</v>
       </c>
-      <c r="D2" t="s">
-        <v>7</v>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>https://assets-prd-spr.unataops.com/web/product_small/8fc77215a3ec068000e57b3e1fd5d3b7a46527ce.jpg</t>
+        </is>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Able to apply prices and links to sheet now. Need to fix some scraping location issues
</commit_message>
<xml_diff>
--- a/Grocery List.xlsx
+++ b/Grocery List.xlsx
@@ -1,36 +1,81 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25427"/>
+  <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Sync\Shared Folder\Groceries and Takeout\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D0BFB41-DE26-4096-8C48-0E11870395EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="18570" yWindow="2130" windowWidth="17295" windowHeight="15345" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sprouts" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="Hy-Vee" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="Sprouts" sheetId="1" r:id="rId1"/>
+    <sheet name="Hy-Vee" sheetId="2" r:id="rId2"/>
   </sheets>
-  <definedNames/>
-  <calcPr calcId="0" fullCalcOnLoad="1"/>
+  <definedNames>
+    <definedName name="Quantity" localSheetId="0">Sprouts!$A:$A</definedName>
+    <definedName name="Quantity">Sprouts!$A:$A</definedName>
+  </definedNames>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="10">
+  <si>
+    <t>Quantity</t>
+  </si>
+  <si>
+    <t>Item</t>
+  </si>
+  <si>
+    <t>Price</t>
+  </si>
+  <si>
+    <t>Image Link</t>
+  </si>
+  <si>
+    <t>Notes</t>
+  </si>
+  <si>
+    <t>Image</t>
+  </si>
+  <si>
+    <t>Pink Lady Apple</t>
+  </si>
+  <si>
+    <t>Pink Lady Apples</t>
+  </si>
+  <si>
+    <t>https://assets-prd-spr.unataops.com/web/product_small/8fc77215a3ec068000e57b3e1fd5d3b7a46527ce.jpg</t>
+  </si>
+  <si>
+    <t>Yellow corn tortillas</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
   </numFmts>
-  <fonts count="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <color theme="1"/>
-      <sz val="11"/>
       <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill/>
+      <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -49,84 +94,25 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="3">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <colors>
-    <indexedColors>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008000"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00808000"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="00C0C0C0"/>
-      <rgbColor rgb="00808080"/>
-      <rgbColor rgb="009999FF"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00FFFFCC"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00660066"/>
-      <rgbColor rgb="00FF8080"/>
-      <rgbColor rgb="000066CC"/>
-      <rgbColor rgb="00CCCCFF"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="0000CCFF"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00CCFFCC"/>
-      <rgbColor rgb="00FFFF99"/>
-      <rgbColor rgb="0099CCFF"/>
-      <rgbColor rgb="00FF99CC"/>
-      <rgbColor rgb="00CC99FF"/>
-      <rgbColor rgb="00FFCC99"/>
-      <rgbColor rgb="003366FF"/>
-      <rgbColor rgb="0033CCCC"/>
-      <rgbColor rgb="0099CC00"/>
-      <rgbColor rgb="00FFCC00"/>
-      <rgbColor rgb="00FF9900"/>
-      <rgbColor rgb="00FF6600"/>
-      <rgbColor rgb="00666699"/>
-      <rgbColor rgb="00969696"/>
-      <rgbColor rgb="00003366"/>
-      <rgbColor rgb="00339966"/>
-      <rgbColor rgb="00003300"/>
-      <rgbColor rgb="00333300"/>
-      <rgbColor rgb="00993300"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00333399"/>
-      <rgbColor rgb="00333333"/>
-    </indexedColors>
-  </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -450,126 +436,107 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:F3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:F50"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col width="16" bestFit="1" customWidth="1" min="2" max="2"/>
-    <col width="10.140625" bestFit="1" customWidth="1" style="1" min="3" max="3"/>
-    <col width="98.85546875" bestFit="1" customWidth="1" min="4" max="4"/>
-    <col width="9.42578125" customWidth="1" min="6" max="6"/>
+    <col min="2" max="2" width="16" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="98.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>Quantity</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>Item</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>Price</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>Image Link</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>Notes</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>Image</t>
-        </is>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
       </c>
     </row>
-    <row r="2" ht="66" customHeight="1">
-      <c r="A2" t="n">
+    <row r="2" spans="1:6" ht="66" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2">
         <v>1</v>
       </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>Pink Lady Apples</t>
-        </is>
-      </c>
-      <c r="C2" s="2" t="n"/>
+      <c r="B2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="2"/>
     </row>
-    <row r="3" ht="66" customHeight="1">
-      <c r="A3" t="n">
+    <row r="3" spans="1:6" ht="66" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3">
         <v>1</v>
       </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>Corn</t>
-        </is>
-      </c>
+      <c r="B3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3"/>
     </row>
-    <row r="4" ht="66" customHeight="1"/>
-    <row r="5" ht="66" customHeight="1"/>
-    <row r="6" ht="66" customHeight="1"/>
-    <row r="7" ht="66" customHeight="1"/>
-    <row r="8" ht="66" customHeight="1"/>
-    <row r="9" ht="66" customHeight="1"/>
-    <row r="10" ht="66" customHeight="1"/>
-    <row r="11" ht="66" customHeight="1"/>
-    <row r="12" ht="66" customHeight="1"/>
-    <row r="13" ht="66" customHeight="1"/>
-    <row r="14" ht="66" customHeight="1"/>
-    <row r="15" ht="66" customHeight="1"/>
-    <row r="16" ht="66" customHeight="1"/>
-    <row r="17" ht="66" customHeight="1"/>
-    <row r="18" ht="66" customHeight="1"/>
-    <row r="19" ht="66" customHeight="1"/>
-    <row r="20" ht="66" customHeight="1"/>
-    <row r="21" ht="66" customHeight="1"/>
-    <row r="22" ht="66" customHeight="1"/>
-    <row r="23" ht="66" customHeight="1"/>
-    <row r="24" ht="66" customHeight="1"/>
-    <row r="25" ht="66" customHeight="1"/>
-    <row r="26" ht="66" customHeight="1"/>
-    <row r="27" ht="66" customHeight="1"/>
-    <row r="28" ht="66" customHeight="1"/>
-    <row r="29" ht="66" customHeight="1"/>
-    <row r="30" ht="66" customHeight="1"/>
-    <row r="31" ht="66" customHeight="1"/>
-    <row r="32" ht="66" customHeight="1"/>
-    <row r="33" ht="66" customHeight="1"/>
-    <row r="34" ht="66" customHeight="1"/>
-    <row r="35" ht="66" customHeight="1"/>
-    <row r="36" ht="66" customHeight="1"/>
-    <row r="37" ht="66" customHeight="1"/>
-    <row r="38" ht="66" customHeight="1"/>
-    <row r="39" ht="66" customHeight="1"/>
-    <row r="40" ht="66" customHeight="1"/>
-    <row r="41" ht="66" customHeight="1"/>
-    <row r="42" ht="66" customHeight="1"/>
-    <row r="43" ht="66" customHeight="1"/>
-    <row r="44" ht="66" customHeight="1"/>
-    <row r="45" ht="66" customHeight="1"/>
-    <row r="46" ht="66" customHeight="1"/>
-    <row r="47" ht="66" customHeight="1"/>
-    <row r="48" ht="66" customHeight="1"/>
-    <row r="49" ht="66" customHeight="1"/>
-    <row r="50" ht="66" customHeight="1"/>
+    <row r="4" spans="1:6" ht="66" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="5" spans="1:6" ht="66" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="6" spans="1:6" ht="66" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="7" spans="1:6" ht="66" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="8" spans="1:6" ht="66" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="9" spans="1:6" ht="66" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="10" spans="1:6" ht="66" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="11" spans="1:6" ht="66" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="12" spans="1:6" ht="66" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="13" spans="1:6" ht="66" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="14" spans="1:6" ht="66" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="15" spans="1:6" ht="66" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="16" spans="1:6" ht="66" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="17" ht="66" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="18" ht="66" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="19" ht="66" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="20" ht="66" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="21" ht="66" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="22" ht="66" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="23" ht="66" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="24" ht="66" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="25" ht="66" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="26" ht="66" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="27" ht="66" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="28" ht="66" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="29" ht="66" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="30" ht="66" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="31" ht="66" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="32" ht="66" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="33" ht="66" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="34" ht="66" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="35" ht="66" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="36" ht="66" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="37" ht="66" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="38" ht="66" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="39" ht="66" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="40" ht="66" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="41" ht="66" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="42" ht="66" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="43" ht="66" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="44" ht="66" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="45" ht="66" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="46" ht="66" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="47" ht="66" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="48" ht="66" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="49" ht="66" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="50" ht="66" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait"/>
@@ -577,71 +544,51 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col width="9.28515625" customWidth="1" min="3" max="3"/>
-    <col width="98.85546875" bestFit="1" customWidth="1" min="4" max="4"/>
+    <col min="3" max="3" width="9.28515625" customWidth="1"/>
+    <col min="4" max="4" width="98.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="41.25" customHeight="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>Quantity</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>Item</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>Price</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>Image Link</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>Notes</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>Image</t>
-        </is>
+    <row r="1" spans="1:6" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" t="n">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2">
         <v>1</v>
       </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>Pink Lady Apples</t>
-        </is>
-      </c>
-      <c r="C2" s="2" t="n">
+      <c r="B2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="2">
         <v>0.6</v>
       </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>https://assets-prd-spr.unataops.com/web/product_small/8fc77215a3ec068000e57b3e1fd5d3b7a46527ce.jpg</t>
-        </is>
+      <c r="D2" t="s">
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Change wait conditions for scraping
</commit_message>
<xml_diff>
--- a/Grocery List.xlsx
+++ b/Grocery List.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Sync\Shared Folder\Groceries and Takeout\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D0BFB41-DE26-4096-8C48-0E11870395EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3EC85A24-8029-4D81-803E-49F45198773D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="11">
   <si>
     <t>Quantity</t>
   </si>
@@ -55,6 +55,9 @@
   </si>
   <si>
     <t>Yellow corn tortillas</t>
+  </si>
+  <si>
+    <t>Cranberries</t>
   </si>
 </sst>
 </file>
@@ -441,7 +444,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B3" sqref="B3"/>
+      <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -490,7 +493,14 @@
       </c>
       <c r="C3"/>
     </row>
-    <row r="4" spans="1:6" ht="66" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="4" spans="1:6" ht="66" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>1</v>
+      </c>
+      <c r="B4" t="s">
+        <v>10</v>
+      </c>
+    </row>
     <row r="5" spans="1:6" ht="66" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="6" spans="1:6" ht="66" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="7" spans="1:6" ht="66" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Add test file for debugging
</commit_message>
<xml_diff>
--- a/Grocery List.xlsx
+++ b/Grocery List.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25427"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Sync\Shared Folder\Groceries and Takeout\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\miche\PycharmProjects\GroceryApp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58B029E4-3DD6-4847-8AD4-74199976034A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE14E50B-5141-4A6B-9DB8-696B33540E9E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2508" yWindow="1272" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sprouts" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="10">
   <si>
     <t>Quantity</t>
   </si>
@@ -55,9 +55,6 @@
   </si>
   <si>
     <t>Yellow corn tortillas</t>
-  </si>
-  <si>
-    <t>Cranberries</t>
   </si>
 </sst>
 </file>
@@ -444,18 +441,18 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
+      <selection pane="bottomLeft" activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="18.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="98.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.42578125" customWidth="1"/>
+    <col min="2" max="2" width="18.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="98.88671875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -475,7 +472,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="66" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" ht="66" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -484,7 +481,7 @@
       </c>
       <c r="C2" s="2"/>
     </row>
-    <row r="3" spans="1:6" ht="66" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" ht="66" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>1</v>
       </c>
@@ -493,60 +490,53 @@
       </c>
       <c r="C3"/>
     </row>
-    <row r="4" spans="1:6" ht="66" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>1</v>
-      </c>
-      <c r="B4" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" ht="66" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="6" spans="1:6" ht="66" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="7" spans="1:6" ht="66" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="8" spans="1:6" ht="66" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="9" spans="1:6" ht="66" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="10" spans="1:6" ht="66" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="11" spans="1:6" ht="66" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="12" spans="1:6" ht="66" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="13" spans="1:6" ht="66" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="14" spans="1:6" ht="66" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="15" spans="1:6" ht="66" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="16" spans="1:6" ht="66" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="17" ht="66" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="18" ht="66" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="19" ht="66" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="20" ht="66" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="21" ht="66" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="22" ht="66" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="23" ht="66" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="24" ht="66" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="25" ht="66" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="26" ht="66" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="27" ht="66" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="28" ht="66" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="29" ht="66" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="30" ht="66" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="31" ht="66" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="32" ht="66" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="33" ht="66" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="34" ht="66" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="35" ht="66" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="36" ht="66" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="37" ht="66" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="38" ht="66" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="39" ht="66" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="40" ht="66" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="41" ht="66" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="42" ht="66" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="43" ht="66" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="44" ht="66" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="45" ht="66" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="46" ht="66" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="47" ht="66" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="48" ht="66" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="49" ht="66" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="50" ht="66" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="4" spans="1:6" ht="66" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="5" spans="1:6" ht="66" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="6" spans="1:6" ht="66" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="7" spans="1:6" ht="66" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="8" spans="1:6" ht="66" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="9" spans="1:6" ht="66" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="10" spans="1:6" ht="66" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="11" spans="1:6" ht="66" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="12" spans="1:6" ht="66" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="13" spans="1:6" ht="66" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="14" spans="1:6" ht="66" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="15" spans="1:6" ht="66" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="16" spans="1:6" ht="66" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="17" ht="66" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="18" ht="66" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="19" ht="66" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="20" ht="66" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="21" ht="66" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="22" ht="66" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="23" ht="66" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="24" ht="66" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="25" ht="66" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="26" ht="66" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="27" ht="66" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="28" ht="66" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="29" ht="66" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="30" ht="66" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="31" ht="66" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="32" ht="66" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="33" ht="66" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="34" ht="66" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="35" ht="66" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="36" ht="66" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="37" ht="66" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="38" ht="66" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="39" ht="66" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="40" ht="66" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="41" ht="66" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="42" ht="66" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="43" ht="66" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="44" ht="66" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="45" ht="66" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="46" ht="66" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="47" ht="66" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="48" ht="66" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="49" ht="66" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="50" ht="66" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait"/>
@@ -561,13 +551,13 @@
       <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="9.28515625" customWidth="1"/>
-    <col min="4" max="4" width="98.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.33203125" customWidth="1"/>
+    <col min="4" max="4" width="98.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" ht="41.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -587,7 +577,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>

</xml_diff>

<commit_message>
Experimenting with changes of locations and methods in order to solve the following products searches
</commit_message>
<xml_diff>
--- a/Grocery List.xlsx
+++ b/Grocery List.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25427"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\miche\PycharmProjects\GroceryApp\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Sync\Shared Folder\Groceries and Takeout\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE14E50B-5141-4A6B-9DB8-696B33540E9E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7871EB6B-9896-456F-ABD2-ABCB13AC5C21}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2508" yWindow="1272" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="21105" yWindow="1590" windowWidth="17295" windowHeight="15345" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sprouts" sheetId="1" r:id="rId1"/>
@@ -437,22 +437,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F50"/>
+  <dimension ref="A1:F49"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D3" sqref="D3"/>
+      <selection pane="bottomLeft" activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="18.88671875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="98.88671875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.44140625" customWidth="1"/>
+    <col min="2" max="2" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="98.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -472,7 +472,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="66" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" ht="66" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -481,7 +481,7 @@
       </c>
       <c r="C2" s="2"/>
     </row>
-    <row r="3" spans="1:6" ht="66" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" ht="66" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1</v>
       </c>
@@ -490,53 +490,52 @@
       </c>
       <c r="C3"/>
     </row>
-    <row r="4" spans="1:6" ht="66" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="5" spans="1:6" ht="66" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="6" spans="1:6" ht="66" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="7" spans="1:6" ht="66" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="8" spans="1:6" ht="66" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="9" spans="1:6" ht="66" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="10" spans="1:6" ht="66" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="11" spans="1:6" ht="66" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="12" spans="1:6" ht="66" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="13" spans="1:6" ht="66" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="14" spans="1:6" ht="66" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="15" spans="1:6" ht="66" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="16" spans="1:6" ht="66" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="17" ht="66" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="18" ht="66" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="19" ht="66" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="20" ht="66" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="21" ht="66" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="22" ht="66" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="23" ht="66" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="24" ht="66" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="25" ht="66" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="26" ht="66" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="27" ht="66" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="28" ht="66" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="29" ht="66" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="30" ht="66" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="31" ht="66" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="32" ht="66" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="33" ht="66" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="34" ht="66" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="35" ht="66" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="36" ht="66" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="37" ht="66" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="38" ht="66" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="39" ht="66" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="40" ht="66" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="41" ht="66" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="42" ht="66" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="43" ht="66" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="44" ht="66" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="45" ht="66" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="46" ht="66" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="47" ht="66" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="48" ht="66" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="49" ht="66" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="50" ht="66" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="4" spans="1:6" ht="66" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="5" spans="1:6" ht="66" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="6" spans="1:6" ht="66" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="7" spans="1:6" ht="66" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="8" spans="1:6" ht="66" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="9" spans="1:6" ht="66" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="10" spans="1:6" ht="66" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="11" spans="1:6" ht="66" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="12" spans="1:6" ht="66" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="13" spans="1:6" ht="66" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="14" spans="1:6" ht="66" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="15" spans="1:6" ht="66" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="16" spans="1:6" ht="66" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="17" ht="66" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="18" ht="66" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="19" ht="66" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="20" ht="66" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="21" ht="66" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="22" ht="66" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="23" ht="66" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="24" ht="66" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="25" ht="66" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="26" ht="66" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="27" ht="66" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="28" ht="66" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="29" ht="66" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="30" ht="66" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="31" ht="66" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="32" ht="66" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="33" ht="66" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="34" ht="66" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="35" ht="66" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="36" ht="66" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="37" ht="66" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="38" ht="66" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="39" ht="66" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="40" ht="66" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="41" ht="66" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="42" ht="66" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="43" ht="66" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="44" ht="66" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="45" ht="66" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="46" ht="66" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="47" ht="66" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="48" ht="66" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="49" ht="66" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait"/>
@@ -551,13 +550,13 @@
       <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="9.33203125" customWidth="1"/>
-    <col min="4" max="4" width="98.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.28515625" customWidth="1"/>
+    <col min="4" max="4" width="98.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="41.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -577,7 +576,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>

</xml_diff>